<commit_message>
Manna Drain mostly Done
</commit_message>
<xml_diff>
--- a/Screweled-Gantt.xlsx
+++ b/Screweled-Gantt.xlsx
@@ -220,10 +220,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.2695856758141958E-2"/>
-          <c:y val="2.9545454545454545E-2"/>
-          <c:w val="0.82531161803857633"/>
-          <c:h val="0.91806442376521091"/>
+          <c:x val="4.9152549781370521E-2"/>
+          <c:y val="4.5454545454545452E-3"/>
+          <c:w val="0.82531161803857656"/>
+          <c:h val="0.9180644237652108"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -366,7 +366,7 @@
                   <c:v>40911</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40921</c:v>
+                  <c:v>40925</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40913</c:v>
@@ -387,7 +387,7 @@
                   <c:v>40911</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40921</c:v>
+                  <c:v>40926</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>40913</c:v>
@@ -402,40 +402,40 @@
                   <c:v>40916</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40919</c:v>
+                  <c:v>40926</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40919</c:v>
+                  <c:v>40926</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40919</c:v>
+                  <c:v>40926</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40919</c:v>
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40920</c:v>
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40920</c:v>
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>40919</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>40914</c:v>
+                  <c:v>40927</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>40913</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>40920</c:v>
+                  <c:v>40928</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>40915</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>40921</c:v>
+                  <c:v>40928</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>40919</c:v>
@@ -447,10 +447,10 @@
                   <c:v>40913</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40922</c:v>
+                  <c:v>40928</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>40921</c:v>
+                  <c:v>40928</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>40910</c:v>
@@ -596,7 +596,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -617,7 +617,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -653,7 +653,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>1</c:v>
@@ -826,7 +826,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -847,7 +847,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -883,7 +883,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>0</c:v>
@@ -926,24 +926,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="48390528"/>
-        <c:axId val="48392064"/>
+        <c:axId val="62481152"/>
+        <c:axId val="62482688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48390528"/>
+        <c:axId val="62481152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48392064"/>
+        <c:crossAx val="62482688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="48392064"/>
+        <c:axId val="62482688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +951,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48390528"/>
+        <c:crossAx val="62481152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -964,8 +964,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.8704277704821286"/>
           <c:y val="0.39102732087101488"/>
-          <c:w val="9.0123953179762448E-2"/>
-          <c:h val="0.10922308279491406"/>
+          <c:w val="9.0123953179762475E-2"/>
+          <c:h val="0.10922308279491408"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1326,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD42"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A3" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1371,13 +1371,13 @@
         <v>24</v>
       </c>
       <c r="B3" s="2">
-        <v>40921</v>
+        <v>40925</v>
       </c>
       <c r="C3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:16384" s="5" customFormat="1">
@@ -1469,13 +1469,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="2">
-        <v>40921</v>
+        <v>40926</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16384" s="5" customFormat="1">
@@ -1539,7 +1539,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="2">
-        <v>40919</v>
+        <v>40926</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1553,7 +1553,7 @@
         <v>29</v>
       </c>
       <c r="B16" s="2">
-        <v>40919</v>
+        <v>40926</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1567,7 +1567,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="2">
-        <v>40919</v>
+        <v>40926</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>31</v>
       </c>
       <c r="B18" s="2">
-        <v>40919</v>
+        <v>40927</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -1595,7 +1595,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="2">
-        <v>40920</v>
+        <v>40927</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -1609,7 +1609,7 @@
         <v>37</v>
       </c>
       <c r="B20" s="2">
-        <v>40920</v>
+        <v>40927</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1637,13 +1637,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="2">
-        <v>40914</v>
+        <v>40927</v>
       </c>
       <c r="C22" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:16384" s="5" customFormat="1">
@@ -1665,7 +1665,7 @@
         <v>32</v>
       </c>
       <c r="B24" s="2">
-        <v>40920</v>
+        <v>40928</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -1693,7 +1693,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="2">
-        <v>40921</v>
+        <v>40928</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1749,7 +1749,7 @@
         <v>42</v>
       </c>
       <c r="B30" s="2">
-        <v>40922</v>
+        <v>40928</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>39</v>
       </c>
       <c r="B31" s="2">
-        <v>40921</v>
+        <v>40928</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Added throttle for multiplier, turned it down 75%
</commit_message>
<xml_diff>
--- a/Screweled-Gantt.xlsx
+++ b/Screweled-Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="8370"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15450" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Start Date</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>CW-7</t>
+  </si>
+  <si>
+    <t>CO-18</t>
+  </si>
+  <si>
+    <t>CL-4</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -194,6 +200,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -251,9 +258,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>CL-1</c:v>
                 </c:pt>
@@ -264,93 +271,99 @@
                   <c:v>CL-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>CL-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>CO-1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>CO-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>CO-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>CO-4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>CO-5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>CO-6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>CO-7</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>CO-8</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>CO-9</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>CO-10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>CO-11</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>CO-12</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>CO-13</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>CO-14</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>CO-15</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>CO-16</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>CO-17</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
+                  <c:v>CO-18</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>LF-1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>LF-2</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>LF-3</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>LF-4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>LF-5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>LF-6</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>CW-1-5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>CW-6</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>CW-7</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>SW-1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>IS-3.1</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>IS-1</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>IS-3</c:v>
                 </c:pt>
               </c:strCache>
@@ -358,10 +371,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$34</c:f>
+              <c:f>Data!$B$2:$B$36</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>40911</c:v>
                 </c:pt>
@@ -372,25 +385,25 @@
                   <c:v>40913</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>40932</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>40911</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>40916</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>40911</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>40914</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>40911</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>40926</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40913</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>40913</c:v>
@@ -399,66 +412,72 @@
                   <c:v>40913</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>40913</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>40916</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>40926</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>40926</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40926</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40927</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40927</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40927</c:v>
+                  <c:v>40930</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>40930</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>40919</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>40927</c:v>
-                </c:pt>
                 <c:pt idx="21">
+                  <c:v>40929</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>40930</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>40913</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>40928</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
+                  <c:v>40930</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>40915</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>40928</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
+                  <c:v>40931</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>40919</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>40910</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>40913</c:v>
                 </c:pt>
-                <c:pt idx="28">
-                  <c:v>40928</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>40928</c:v>
-                </c:pt>
                 <c:pt idx="30">
+                  <c:v>40931</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40929</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>40910</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>40910</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>40910</c:v>
                 </c:pt>
               </c:numCache>
@@ -481,9 +500,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>CL-1</c:v>
                 </c:pt>
@@ -494,93 +513,99 @@
                   <c:v>CL-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>CL-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>CO-1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>CO-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>CO-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>CO-4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>CO-5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>CO-6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>CO-7</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>CO-8</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>CO-9</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>CO-10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>CO-11</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>CO-12</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>CO-13</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>CO-14</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>CO-15</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>CO-16</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>CO-17</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
+                  <c:v>CO-18</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>LF-1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>LF-2</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>LF-3</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>LF-4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>LF-5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>LF-6</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>CW-1-5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>CW-6</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>CW-7</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>SW-1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>IS-3.1</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>IS-1</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>IS-3</c:v>
                 </c:pt>
               </c:strCache>
@@ -588,10 +613,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$34</c:f>
+              <c:f>Data!$C$2:$C$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -602,7 +627,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -617,7 +642,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -629,11 +654,11 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
@@ -641,7 +666,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -650,13 +675,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -671,24 +696,30 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="31">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -711,9 +742,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$34</c:f>
+              <c:f>Data!$A$2:$A$36</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>CL-1</c:v>
                 </c:pt>
@@ -724,93 +755,99 @@
                   <c:v>CL-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>CL-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>CO-1</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>CO-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>CO-3</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>CO-4</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>CO-5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>CO-6</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>CO-7</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>CO-8</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>CO-9</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>CO-10</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>CO-11</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>CO-12</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>CO-13</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>CO-14</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>CO-15</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>CO-16</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>CO-17</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
+                  <c:v>CO-18</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>LF-1</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="23">
                   <c:v>LF-2</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>LF-3</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>LF-4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>LF-5</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
                   <c:v>LF-6</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="28">
                   <c:v>CW-1-5</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="29">
                   <c:v>CW-6</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>CW-7</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="31">
                   <c:v>SW-1</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="32">
                   <c:v>IS-3.1</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="33">
                   <c:v>IS-1</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="34">
                   <c:v>IS-3</c:v>
                 </c:pt>
               </c:strCache>
@@ -818,10 +855,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$34</c:f>
+              <c:f>Data!$D$2:$D$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -832,7 +869,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -862,7 +899,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -871,7 +908,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -880,13 +917,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1</c:v>
@@ -895,30 +932,36 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="27">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="31">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -989,7 +1032,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10752667" cy="5588000"/>
+    <xdr:ext cx="10752667" cy="5894917"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1324,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD42"/>
+  <dimension ref="A1:XFD44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1394,26 +1437,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" customFormat="1">
+    <row r="5" spans="1:16384" s="8" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
-        <v>40911</v>
+        <v>40932</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16384" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>40916</v>
+        <v>40911</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1422,12 +1465,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" s="4" customFormat="1">
+    <row r="7" spans="1:16384" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>40911</v>
+        <v>40916</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1438,10 +1481,10 @@
     </row>
     <row r="8" spans="1:16384" s="4" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2">
-        <v>40914</v>
+        <v>40911</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1452,10 +1495,10 @@
     </row>
     <row r="9" spans="1:16384" s="4" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
-        <v>40911</v>
+        <v>40914</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1466,24 +1509,24 @@
     </row>
     <row r="10" spans="1:16384" s="4" customFormat="1">
       <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>40911</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16384" s="4" customFormat="1">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <v>40926</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16384" s="5" customFormat="1">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2">
-        <v>40913</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1494,7 +1537,7 @@
     </row>
     <row r="12" spans="1:16384" s="5" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>40913</v>
@@ -1508,7 +1551,7 @@
     </row>
     <row r="13" spans="1:16384" s="5" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>40913</v>
@@ -1522,13 +1565,13 @@
     </row>
     <row r="14" spans="1:16384" s="5" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
-        <v>40916</v>
+        <v>40913</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -1536,24 +1579,24 @@
     </row>
     <row r="15" spans="1:16384" s="5" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2">
-        <v>40926</v>
+        <v>40916</v>
       </c>
       <c r="C15" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16384" s="5" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
-        <v>40926</v>
+        <v>40929</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1564,10 +1607,10 @@
     </row>
     <row r="17" spans="1:16384" s="5" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
-        <v>40926</v>
+        <v>40929</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1578,38 +1621,38 @@
     </row>
     <row r="18" spans="1:16384" s="5" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2">
-        <v>40927</v>
+        <v>40929</v>
       </c>
       <c r="C18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:16384" s="5" customFormat="1">
       <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16384" s="5" customFormat="1">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2">
-        <v>40927</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16384" s="7" customFormat="1">
-      <c r="A20" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="B20" s="2">
-        <v>40927</v>
+        <v>40930</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1620,52 +1663,52 @@
     </row>
     <row r="21" spans="1:16384" s="7" customFormat="1">
       <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>40930</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16384" s="7" customFormat="1">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="2">
         <v>40919</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16384" s="4" customFormat="1">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16384" s="8" customFormat="1">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16384" s="4" customFormat="1">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="2">
-        <v>40927</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16384" s="5" customFormat="1">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
-        <v>40913</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16384" s="5" customFormat="1">
-      <c r="A24" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="B24" s="2">
-        <v>40928</v>
+        <v>40930</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -1676,10 +1719,10 @@
     </row>
     <row r="25" spans="1:16384" s="5" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B25" s="2">
-        <v>40915</v>
+        <v>40913</v>
       </c>
       <c r="C25" s="1">
         <v>1</v>
@@ -1690,149 +1733,177 @@
     </row>
     <row r="26" spans="1:16384" s="5" customFormat="1">
       <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="2">
+        <v>40930</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16384" s="5" customFormat="1">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="2">
+        <v>40915</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16384" s="5" customFormat="1">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="2">
-        <v>40928</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="B28" s="2">
+        <v>40931</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:16384" s="6" customFormat="1">
-      <c r="A27" s="1" t="s">
+    <row r="29" spans="1:16384" s="6" customFormat="1">
+      <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B29" s="2">
         <v>40919</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16384" s="4" customFormat="1">
-      <c r="A28" s="1" t="s">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16384" s="4" customFormat="1">
+      <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B30" s="2">
         <v>40910</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C30" s="1">
         <v>4</v>
       </c>
-      <c r="D28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16384" s="5" customFormat="1">
-      <c r="A29" s="1" t="s">
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16384" s="5" customFormat="1">
+      <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B31" s="2">
         <v>40913</v>
       </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16384" s="7" customFormat="1">
-      <c r="A30" s="1" t="s">
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16384" s="7" customFormat="1">
+      <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="2">
-        <v>40928</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="B32" s="2">
+        <v>40931</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:16384" s="7" customFormat="1">
-      <c r="A31" s="1" t="s">
+    <row r="33" spans="1:16384" s="7" customFormat="1">
+      <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="2">
-        <v>40928</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16384" s="4" customFormat="1">
-      <c r="A32" s="1" t="s">
+      <c r="B33" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16384" s="4" customFormat="1">
+      <c r="A34" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B32" s="2">
-        <v>40910</v>
-      </c>
-      <c r="C32" s="1">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16384" s="3" customFormat="1">
-      <c r="A33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="2">
-        <v>40910</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16384" customFormat="1">
-      <c r="A34" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B34" s="2">
         <v>40910</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16384" customFormat="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:16384" customFormat="1"/>
-    <row r="37" spans="1:16384" customFormat="1"/>
+    <row r="35" spans="1:16384" s="3" customFormat="1">
+      <c r="A35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2">
+        <v>40910</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16384" customFormat="1">
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2">
+        <v>40910</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16384" customFormat="1">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+    </row>
     <row r="38" spans="1:16384" customFormat="1"/>
     <row r="39" spans="1:16384" customFormat="1"/>
     <row r="40" spans="1:16384" customFormat="1"/>
     <row r="41" spans="1:16384" customFormat="1"/>
     <row r="42" spans="1:16384" customFormat="1"/>
+    <row r="43" spans="1:16384" customFormat="1"/>
+    <row r="44" spans="1:16384" customFormat="1"/>
   </sheetData>
   <sortState ref="A2:D17">
     <sortCondition ref="A2:A17"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A37:D37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Manna drain and 5 rage explosive jewels added
</commit_message>
<xml_diff>
--- a/Screweled-Gantt.xlsx
+++ b/Screweled-Gantt.xlsx
@@ -12,12 +12,12 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1:Q31"/>
+  <oleSize ref="A9:O40"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Start Date</t>
   </si>
@@ -167,6 +167,45 @@
   </si>
   <si>
     <t>LF-8</t>
+  </si>
+  <si>
+    <t>IS-3.1.1</t>
+  </si>
+  <si>
+    <t>CO-1.1</t>
+  </si>
+  <si>
+    <t>CO-2.1</t>
+  </si>
+  <si>
+    <t>CO-3.1</t>
+  </si>
+  <si>
+    <t>CO-4.1</t>
+  </si>
+  <si>
+    <t>CO-5.1</t>
+  </si>
+  <si>
+    <t>CO-7.1</t>
+  </si>
+  <si>
+    <t>CO-8.1</t>
+  </si>
+  <si>
+    <t>CO-9.1</t>
+  </si>
+  <si>
+    <t>CO-10.1</t>
+  </si>
+  <si>
+    <t>CO-13.1</t>
+  </si>
+  <si>
+    <t>LF-2.1</t>
+  </si>
+  <si>
+    <t>CW-2.1</t>
   </si>
 </sst>
 </file>
@@ -208,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -216,6 +255,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -243,10 +283,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.9152549781370514E-2"/>
-          <c:y val="4.5454545454545461E-3"/>
-          <c:w val="0.82531161803857689"/>
-          <c:h val="0.91806442376521069"/>
+          <c:x val="5.5058061409322914E-2"/>
+          <c:y val="4.545441437088937E-3"/>
+          <c:w val="0.82531161803857711"/>
+          <c:h val="0.91806442376521058"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -274,56 +314,56 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$26</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>LF-4</c:v>
+                  <c:v>CL-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CO-2</c:v>
+                  <c:v>CO-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CO-10</c:v>
+                  <c:v>CO-13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CO-17</c:v>
+                  <c:v>CO-18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LF-6</c:v>
+                  <c:v>SW-1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>CL-2</c:v>
+                  <c:v>LF-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>CO-6</c:v>
+                  <c:v>CW-9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>CW-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>IS-3.1.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>CO-11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>CO-12</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>CO-13</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>CO-14</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>CO-18</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>SW-1</c:v>
+                  <c:v>CO-15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>CO-15</c:v>
+                  <c:v>CO-16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>CO-16</c:v>
+                  <c:v>LF-1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>LF-1</c:v>
+                  <c:v>LF-2.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>LF-3</c:v>
@@ -332,91 +372,115 @@
                   <c:v>LF-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>LF-7</c:v>
+                  <c:v>CO-3.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>CO-4.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>CO-5.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>CO-7.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>CO-8.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>CO-9.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>CO-1.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>LF-8</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>CW-7</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>CW-8</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>CW-9</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="27">
                   <c:v>CL-4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
+                  <c:v>CW-2.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>CW-10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>CO-2.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>CO-10.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>CO-13.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$26</c:f>
+              <c:f>Data!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>40915</c:v>
+                  <c:v>40925</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40916</c:v>
+                  <c:v>40926</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40916</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40919</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40919</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40925</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40926</c:v>
+                  <c:v>40929</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40932</c:v>
+                  <c:v>40930</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>40932</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40929</c:v>
+                  <c:v>40936</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>40936</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40936</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40936</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40937</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>40932</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>40929</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>40929</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>40932</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>40933</c:v>
-                </c:pt>
                 <c:pt idx="15">
-                  <c:v>40933</c:v>
+                  <c:v>40934</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40933</c:v>
+                  <c:v>40937</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>40933</c:v>
+                  <c:v>40937</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>40929</c:v>
+                  <c:v>40934</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>40934</c:v>
@@ -425,16 +489,40 @@
                   <c:v>40934</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>40930</c:v>
+                  <c:v>40934</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>40929</c:v>
+                  <c:v>40934</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>40934</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>40932</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>40937</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>40938</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>40934</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>40938</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>40935</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40935</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -456,56 +544,56 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$26</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>LF-4</c:v>
+                  <c:v>CL-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CO-2</c:v>
+                  <c:v>CO-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CO-10</c:v>
+                  <c:v>CO-13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CO-17</c:v>
+                  <c:v>CO-18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LF-6</c:v>
+                  <c:v>SW-1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>CL-2</c:v>
+                  <c:v>LF-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>CO-6</c:v>
+                  <c:v>CW-9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>CW-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>IS-3.1.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>CO-11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>CO-12</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>CO-13</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>CO-14</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>CO-18</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>SW-1</c:v>
+                  <c:v>CO-15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>CO-15</c:v>
+                  <c:v>CO-16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>CO-16</c:v>
+                  <c:v>LF-1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>LF-1</c:v>
+                  <c:v>LF-2.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>LF-3</c:v>
@@ -514,109 +602,157 @@
                   <c:v>LF-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>LF-7</c:v>
+                  <c:v>CO-3.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>CO-4.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>CO-5.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>CO-7.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>CO-8.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>CO-9.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>CO-1.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>LF-8</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>CW-7</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>CW-8</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>CW-9</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="27">
                   <c:v>CL-4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
+                  <c:v>CW-2.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>CW-10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>CO-2.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>CO-10.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>CO-13.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$26</c:f>
+              <c:f>Data!$C$2:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="31">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -638,56 +774,56 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$26</c:f>
+              <c:f>Data!$A$2:$A$34</c:f>
               <c:strCache>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
-                  <c:v>LF-4</c:v>
+                  <c:v>CL-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CO-2</c:v>
+                  <c:v>CO-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>CO-10</c:v>
+                  <c:v>CO-13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CO-17</c:v>
+                  <c:v>CO-18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LF-6</c:v>
+                  <c:v>SW-1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>CL-2</c:v>
+                  <c:v>LF-7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>CO-6</c:v>
+                  <c:v>CW-9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>CW-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>IS-3.1.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>CO-11</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>CO-12</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>CO-13</c:v>
-                </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>CO-14</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>CO-18</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>SW-1</c:v>
+                  <c:v>CO-15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>CO-15</c:v>
+                  <c:v>CO-16</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>CO-16</c:v>
+                  <c:v>LF-1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>LF-1</c:v>
+                  <c:v>LF-2.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>LF-3</c:v>
@@ -696,35 +832,59 @@
                   <c:v>LF-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>LF-7</c:v>
+                  <c:v>CO-3.1</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>CO-4.1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>CO-5.1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>CO-7.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>CO-8.1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>CO-9.1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>CO-1.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>LF-8</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="26">
                   <c:v>CW-7</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>CW-8</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>CW-9</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="27">
                   <c:v>CL-4</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="28">
+                  <c:v>CW-2.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>CW-10</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>CO-2.1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>CO-10.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>CO-13.1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$26</c:f>
+              <c:f>Data!$D$2:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -747,31 +907,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -783,46 +943,70 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="68668416"/>
-        <c:axId val="71054080"/>
+        <c:axId val="68198784"/>
+        <c:axId val="68201088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68668416"/>
+        <c:axId val="68198784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71054080"/>
+        <c:crossAx val="68201088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71054080"/>
+        <c:axId val="68201088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +1014,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68668416"/>
+        <c:crossAx val="68198784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -843,8 +1027,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.8704277704821286"/>
           <c:y val="0.39102732087101488"/>
-          <c:w val="9.0123953179762503E-2"/>
-          <c:h val="0.10922308279491411"/>
+          <c:w val="9.0123953179762517E-2"/>
+          <c:h val="0.10922308279491413"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1203,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD49"/>
+  <dimension ref="A1:XFD62"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A9" zoomScale="90" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1231,12 +1415,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="5" customFormat="1">
+    <row r="2" spans="1:16384" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
-        <v>40915</v>
+        <v>40925</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1245,180 +1429,180 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" s="5" customFormat="1">
+    <row r="3" spans="1:16384" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
-        <v>40916</v>
+        <v>40926</v>
       </c>
       <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16384" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16384" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16384" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16384" s="5" customFormat="1">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16384" s="9" customFormat="1">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2">
+        <v>40929</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16384" s="9" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2">
+        <v>40930</v>
+      </c>
+      <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16384" s="5" customFormat="1">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2">
-        <v>40916</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16384" s="5" customFormat="1">
-      <c r="A5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="2">
-        <v>40919</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16384" s="7" customFormat="1">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="2">
-        <v>40919</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16384" s="7" customFormat="1">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2">
-        <v>40925</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16384" s="8" customFormat="1">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2">
-        <v>40926</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16384" s="4" customFormat="1">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2">
-        <v>40932</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
       <c r="D9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16384" s="5" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B10" s="2">
         <v>40932</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16384" s="5" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16384" s="7" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2">
-        <v>40929</v>
+        <v>40936</v>
       </c>
       <c r="C11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16384" s="5" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16384" s="7" customFormat="1">
       <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2">
+        <v>40936</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16384" s="9" customFormat="1">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2">
-        <v>40932</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16384" s="5" customFormat="1">
-      <c r="A13" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="B13" s="2">
-        <v>40929</v>
+        <v>40936</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16384" s="6" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16384" s="8" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
-        <v>40929</v>
+        <v>40936</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16384" s="4" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2">
-        <v>40932</v>
+        <v>40937</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1429,38 +1613,38 @@
     </row>
     <row r="16" spans="1:16384" s="5" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
-        <v>40933</v>
+        <v>40932</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16384" s="7" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16384" s="9" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2">
-        <v>40933</v>
+        <v>40934</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16384" s="8" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16384" s="5" customFormat="1">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2">
-        <v>40933</v>
+        <v>40937</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -1469,12 +1653,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16384" s="8" customFormat="1">
+    <row r="19" spans="1:16384" s="5" customFormat="1">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="2">
-        <v>40933</v>
+        <v>40937</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -1483,12 +1667,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:16384" s="8" customFormat="1">
+    <row r="20" spans="1:16384" s="5" customFormat="1">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2">
-        <v>40929</v>
+        <v>40934</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -1497,54 +1681,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16384" s="8" customFormat="1">
+    <row r="21" spans="1:16384" s="6" customFormat="1">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2">
         <v>40934</v>
       </c>
       <c r="C21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16384" s="8" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16384" s="4" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2">
         <v>40934</v>
       </c>
       <c r="C22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16384" s="7" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16384" s="5" customFormat="1">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2">
-        <v>40930</v>
+        <v>40934</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16384" s="4" customFormat="1">
+    <row r="24" spans="1:16384" s="7" customFormat="1">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B24" s="2">
-        <v>40929</v>
+        <v>40934</v>
       </c>
       <c r="C24" s="1">
         <v>1</v>
@@ -1553,48 +1737,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16384" s="3" customFormat="1">
+    <row r="25" spans="1:16384" s="8" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2">
         <v>40934</v>
       </c>
       <c r="C25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16384" customFormat="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16384" s="8" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2">
         <v>40934</v>
       </c>
       <c r="C26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16384" customFormat="1">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:16384" customFormat="1"/>
-    <row r="29" spans="1:16384" customFormat="1"/>
-    <row r="30" spans="1:16384" customFormat="1"/>
-    <row r="31" spans="1:16384" customFormat="1"/>
-    <row r="32" spans="1:16384" customFormat="1"/>
-    <row r="33" spans="1:16384" customFormat="1"/>
-    <row r="34" spans="1:16384" customFormat="1"/>
-    <row r="35" spans="1:16384" customFormat="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16384" s="8" customFormat="1">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2">
+        <v>40932</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16384" s="8" customFormat="1">
+      <c r="A28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="2">
+        <v>40937</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16384" s="8" customFormat="1">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="2">
+        <v>40938</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16384" s="9" customFormat="1">
+      <c r="A30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="2">
+        <v>40934</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16384" s="7" customFormat="1">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="2">
+        <v>40938</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16384" s="4" customFormat="1">
+      <c r="A32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="2">
+        <v>40935</v>
+      </c>
+      <c r="C32" s="1">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16384" s="3" customFormat="1">
+      <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="2">
+        <v>40935</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16384" customFormat="1">
+      <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="2">
+        <v>40935</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16384" customFormat="1">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+    </row>
     <row r="36" spans="1:16384" customFormat="1"/>
     <row r="37" spans="1:16384" customFormat="1"/>
     <row r="38" spans="1:16384" customFormat="1"/>
@@ -1609,12 +1897,25 @@
     <row r="47" spans="1:16384" customFormat="1"/>
     <row r="48" spans="1:16384" customFormat="1"/>
     <row r="49" spans="1:16384" customFormat="1"/>
+    <row r="50" spans="1:16384" customFormat="1"/>
+    <row r="51" spans="1:16384" customFormat="1"/>
+    <row r="52" spans="1:16384" customFormat="1"/>
+    <row r="53" spans="1:16384" customFormat="1"/>
+    <row r="54" spans="1:16384" customFormat="1"/>
+    <row r="55" spans="1:16384" customFormat="1"/>
+    <row r="56" spans="1:16384" customFormat="1"/>
+    <row r="57" spans="1:16384" customFormat="1"/>
+    <row r="58" spans="1:16384" customFormat="1"/>
+    <row r="59" spans="1:16384" customFormat="1"/>
+    <row r="60" spans="1:16384" customFormat="1"/>
+    <row r="61" spans="1:16384" customFormat="1"/>
+    <row r="62" spans="1:16384" customFormat="1"/>
   </sheetData>
-  <sortState ref="A2:D39">
-    <sortCondition ref="B2:B39"/>
+  <sortState ref="A2:D37">
+    <sortCondition ref="B2:B37"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1623,13 +1924,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD22"/>
+  <dimension ref="A1:XFD27"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16384">
       <c r="A1" s="7" t="s">
@@ -1927,6 +2231,76 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16384">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2">
+        <v>40915</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16384">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2">
+        <v>40916</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16384">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2">
+        <v>40916</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16384">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2">
+        <v>40919</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16384">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="2">
+        <v>40919</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Code clean up, reduced bugs in Contiguous check and isMannable
</commit_message>
<xml_diff>
--- a/Screweled-Gantt.xlsx
+++ b/Screweled-Gantt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="veryHidden" xWindow="-150" yWindow="-480" windowWidth="15690" windowHeight="9060"/>
+    <workbookView visibility="veryHidden" xWindow="0" yWindow="0" windowWidth="15450" windowHeight="8490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="4" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A9:O40"/>
+  <oleSize ref="A9:N39"/>
 </workbook>
 </file>
 
@@ -1041,7 +1041,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1389,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:XFD62"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>

</xml_diff>